<commit_message>
applied RC color themes to excel export
</commit_message>
<xml_diff>
--- a/docs/sample_result.xlsx
+++ b/docs/sample_result.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,11 +27,12 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00002855"/>
       <sz val="16"/>
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00000000"/>
+      <color rgb="00002855"/>
     </font>
     <font>
       <b val="1"/>
@@ -40,8 +41,12 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="002B2926"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -50,26 +55,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E7F3FF"/>
-        <bgColor rgb="00E7F3FF"/>
+        <fgColor rgb="00F1EFEC"/>
+        <bgColor rgb="00F1EFEC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
+        <fgColor rgb="000684BC"/>
+        <bgColor rgb="000684BC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFACD"/>
-        <bgColor rgb="00FFFACD"/>
+        <fgColor rgb="00FF7A00"/>
+        <bgColor rgb="00FF7A00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E6FFE6"/>
-        <bgColor rgb="00E6FFE6"/>
+        <fgColor rgb="00DC3545"/>
+        <bgColor rgb="00DC3545"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE6E6"/>
+        <bgColor rgb="00FFE6E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -82,16 +93,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color rgb="00C8C2B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="00C8C2B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="00C8C2B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00C8C2B4"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -111,13 +130,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -522,7 +544,7 @@
     <row r="2" ht="25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2025-07-02 10:55:51</t>
+          <t>Generated: 2025-07-02 13:09:53</t>
         </is>
       </c>
     </row>
@@ -561,7 +583,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
@@ -572,7 +594,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10%</t>
         </is>
       </c>
     </row>
@@ -583,7 +605,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>79.5</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
@@ -603,7 +625,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" ht="25" customHeight="1">
@@ -642,7 +664,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>SElECT Id FROM Lead WHERE ZI_Employees__c &gt; 1000</t>
+          <t>SELECT Id FROM Lead WHERE ZI_Employees__c &gt; 2000</t>
         </is>
       </c>
     </row>
@@ -654,7 +676,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>28.43s</t>
+          <t>27.51s</t>
         </is>
       </c>
     </row>
@@ -750,12 +772,12 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmYXcUAN</t>
+          <t>00Q2H00002BmaghUAB</t>
         </is>
       </c>
       <c r="B21" s="7" t="inlineStr">
         <is>
-          <t>skwiker@plymouthrock.com</t>
+          <t>david_edelman@edelman-lyon.com</t>
         </is>
       </c>
       <c r="C21" s="7" t="inlineStr">
@@ -765,27 +787,31 @@
       </c>
       <c r="D21" s="7" t="inlineStr">
         <is>
-          <t>Majors</t>
-        </is>
-      </c>
-      <c r="E21" s="7" t="n"/>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="inlineStr">
+        <is>
+          <t>400-4999</t>
+        </is>
+      </c>
       <c r="F21" s="7" t="inlineStr">
         <is>
-          <t>bunkerhillins.com</t>
+          <t>edelman.com</t>
         </is>
       </c>
       <c r="G21" s="7" t="n"/>
       <c r="H21" s="7" t="inlineStr">
         <is>
-          <t>Bunker Hill</t>
+          <t>Daniel J Edelman Holdings Inc</t>
         </is>
       </c>
       <c r="I21" s="7" t="n">
-        <v>1800</v>
+        <v>5610</v>
       </c>
       <c r="J21" s="7" t="inlineStr">
         <is>
-          <t>plymouthrock.com</t>
+          <t>edelman-lyon.com</t>
         </is>
       </c>
       <c r="K21" s="8" t="inlineStr">
@@ -803,26 +829,13 @@
       </c>
       <c r="N21" s="10" t="inlineStr">
         <is>
-          <t>✅ ZI_Company_Name__c matches email domain and Website.
-✅ ZI_Employees__c aligns with 'Majors' segment size range.
-⚠️ LS_Company_Size_Range__c missing, could provide additional context.
-⚠️ Website missing, consider inferring from email domain or external sources.</t>
-        </is>
-      </c>
-      <c r="O21" s="10" t="inlineStr">
-        <is>
-          <t>{
-  "ZI_Company_Name__c": "Plymouth Rock"
-}</t>
-        </is>
-      </c>
-      <c r="P21" s="10" t="inlineStr">
-        <is>
-          <t>{
-  "ZI_Website__c": "plymouthrock.com"
-}</t>
-        </is>
-      </c>
+          <t>✅ ZI_Company_Name__c matches email domain; strong brand alignment.
+⚠️ ZI_Website__c is missing; inferred primary site from email domain.
+✅ ZI_Employees__c consistent with Enterprise segment size range.</t>
+        </is>
+      </c>
+      <c r="O21" s="10" t="inlineStr"/>
+      <c r="P21" s="10" t="inlineStr"/>
       <c r="Q21" s="7" t="inlineStr">
         <is>
           <t>success</t>
@@ -832,12 +845,12 @@
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmYn2UAF</t>
+          <t>00Q2H00002BmapUUAR</t>
         </is>
       </c>
       <c r="B22" s="7" t="inlineStr">
         <is>
-          <t>michael.strouch@cedarpointfinancial.com</t>
+          <t>emily@emilydavisconsulting.com</t>
         </is>
       </c>
       <c r="C22" s="7" t="inlineStr">
@@ -847,27 +860,27 @@
       </c>
       <c r="D22" s="7" t="inlineStr">
         <is>
-          <t>Majors</t>
+          <t>Enterprise</t>
         </is>
       </c>
       <c r="E22" s="7" t="n"/>
       <c r="F22" s="7" t="inlineStr">
         <is>
-          <t>cedarpointfinancial.com</t>
+          <t>emilydavisconsulting.com</t>
         </is>
       </c>
       <c r="G22" s="7" t="n"/>
       <c r="H22" s="7" t="inlineStr">
         <is>
-          <t>Fairfield University</t>
+          <t>Medtronic</t>
         </is>
       </c>
       <c r="I22" s="7" t="n">
-        <v>1477</v>
+        <v>95000</v>
       </c>
       <c r="J22" s="7" t="inlineStr">
         <is>
-          <t>cedarpointfinancial.com</t>
+          <t>emilydavisconsulting.com</t>
         </is>
       </c>
       <c r="K22" s="8" t="inlineStr">
@@ -880,614 +893,616 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M22" s="9" t="n">
-        <v>75</v>
+      <c r="M22" s="11" t="n">
+        <v>50</v>
       </c>
       <c r="N22" s="10" t="inlineStr">
         <is>
-          <t>⚠️ ZI_Company_Name__c 'Fairfield University' conflicts with email domain 'cedarpointfinancial.com'.
-✅ ZI_Employees__c aligns with 'Majors' segment size range.
-✅ Corporate email domain matches Website and ZI_Company_Name__c.</t>
+          <t>⚠️ ZI_Company_Name__c 'Medtronic' conflicts with email domain 'emilydavisconsulting.com'.
+✅ ZI_Employees__c aligns with 'Enterprise' segment size; no size-range conflict.</t>
         </is>
       </c>
       <c r="O22" s="10" t="inlineStr">
-        <is>
-          <t>{
-  "ZI_Company_Name__c": "Cedar Point Financial"
-}</t>
-        </is>
-      </c>
-      <c r="P22" s="10" t="inlineStr"/>
-      <c r="Q22" s="7" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="25" customHeight="1">
-      <c r="A23" s="7" t="inlineStr">
-        <is>
-          <t>00Q2H00002BmYvVUAV</t>
-        </is>
-      </c>
-      <c r="B23" s="7" t="inlineStr">
-        <is>
-          <t>scott.campbell@chicagofed.org</t>
-        </is>
-      </c>
-      <c r="C23" s="7" t="inlineStr">
-        <is>
-          <t>List Purchase</t>
-        </is>
-      </c>
-      <c r="D23" s="7" t="inlineStr">
-        <is>
-          <t>Majors</t>
-        </is>
-      </c>
-      <c r="E23" s="7" t="inlineStr">
-        <is>
-          <t>20-99</t>
-        </is>
-      </c>
-      <c r="F23" s="7" t="inlineStr">
-        <is>
-          <t>www.chicagofed.org</t>
-        </is>
-      </c>
-      <c r="G23" s="7" t="n"/>
-      <c r="H23" s="7" t="inlineStr">
-        <is>
-          <t>Federal Reserve Bank of Chicago</t>
-        </is>
-      </c>
-      <c r="I23" s="7" t="n">
-        <v>1580</v>
-      </c>
-      <c r="J23" s="7" t="inlineStr">
-        <is>
-          <t>chicagofed.org</t>
-        </is>
-      </c>
-      <c r="K23" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L23" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M23" s="11" t="n">
-        <v>90</v>
-      </c>
-      <c r="N23" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain and trusted internal data.
-✅ ZI_Employees__c aligns with the 'large' company segment and internal size range estimate.
-⚠️ Website missing in ZoomInfo enrichment; inferred primary site from trusted internal data.
-✅ No flags raised for incomplete or suspicious enrichment.</t>
-        </is>
-      </c>
-      <c r="O23" s="10" t="inlineStr"/>
-      <c r="P23" s="10" t="inlineStr"/>
-      <c r="Q23" s="7" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="25" customHeight="1">
-      <c r="A24" s="7" t="inlineStr">
-        <is>
-          <t>00Q2H00002BmaghUAB</t>
-        </is>
-      </c>
-      <c r="B24" s="7" t="inlineStr">
-        <is>
-          <t>david_edelman@edelman-lyon.com</t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>List Purchase</t>
-        </is>
-      </c>
-      <c r="D24" s="7" t="inlineStr">
-        <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E24" s="7" t="inlineStr">
-        <is>
-          <t>400-4999</t>
-        </is>
-      </c>
-      <c r="F24" s="7" t="inlineStr">
-        <is>
-          <t>edelman.com</t>
-        </is>
-      </c>
-      <c r="G24" s="7" t="n"/>
-      <c r="H24" s="7" t="inlineStr">
-        <is>
-          <t>Daniel J Edelman Holdings Inc</t>
-        </is>
-      </c>
-      <c r="I24" s="7" t="n">
-        <v>5610</v>
-      </c>
-      <c r="J24" s="7" t="inlineStr">
-        <is>
-          <t>edelman-lyon.com</t>
-        </is>
-      </c>
-      <c r="K24" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L24" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M24" s="9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N24" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain; high brand consistency.
-✅ ZI_Employees__c aligns with LS_Company_Size_Range__c for Enterprise segment.
-⚠️ ZI_Website__c missing; inferred primary site from ZoomInfo enrichment.</t>
-        </is>
-      </c>
-      <c r="O24" s="10" t="inlineStr"/>
-      <c r="P24" s="10" t="inlineStr"/>
-      <c r="Q24" s="7" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="25" customHeight="1">
-      <c r="A25" s="7" t="inlineStr">
-        <is>
-          <t>00Q2H00002BmapUUAR</t>
-        </is>
-      </c>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>emily@emilydavisconsulting.com</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="inlineStr">
-        <is>
-          <t>List Purchase</t>
-        </is>
-      </c>
-      <c r="D25" s="7" t="inlineStr">
-        <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E25" s="7" t="n"/>
-      <c r="F25" s="7" t="inlineStr">
-        <is>
-          <t>emilydavisconsulting.com</t>
-        </is>
-      </c>
-      <c r="G25" s="7" t="n"/>
-      <c r="H25" s="7" t="inlineStr">
-        <is>
-          <t>Medtronic</t>
-        </is>
-      </c>
-      <c r="I25" s="7" t="n">
-        <v>95000</v>
-      </c>
-      <c r="J25" s="7" t="inlineStr">
-        <is>
-          <t>emilydavisconsulting.com</t>
-        </is>
-      </c>
-      <c r="K25" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L25" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M25" s="9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N25" s="10" t="inlineStr">
-        <is>
-          <t>⚠️ ZI_Company_Name__c 'Medtronic' conflicts with email domain 'emilydavisconsulting.com'.
-✅ ZI_Employees__c aligns with 'Enterprise' segment size range.
-✅ ZI_Website__c and Website are both missing, requiring validation.</t>
-        </is>
-      </c>
-      <c r="O25" s="10" t="inlineStr">
         <is>
           <t>{
   "ZI_Company_Name__c": "Emily Davis Consulting"
 }</t>
         </is>
       </c>
-      <c r="P25" s="10" t="inlineStr"/>
-      <c r="Q25" s="7" t="inlineStr">
+      <c r="P22" s="10" t="inlineStr"/>
+      <c r="Q22" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="25" customHeight="1">
-      <c r="A26" s="7" t="inlineStr">
+    <row r="23" ht="25" customHeight="1">
+      <c r="A23" s="7" t="inlineStr">
         <is>
           <t>00Q2H00002BmblPUAR</t>
         </is>
       </c>
-      <c r="B26" s="7" t="inlineStr">
+      <c r="B23" s="7" t="inlineStr">
         <is>
           <t>lori@hatchstaff.com</t>
         </is>
       </c>
-      <c r="C26" s="7" t="inlineStr">
+      <c r="C23" s="7" t="inlineStr">
         <is>
           <t>List Purchase</t>
         </is>
       </c>
-      <c r="D26" s="7" t="inlineStr">
+      <c r="D23" s="7" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E26" s="7" t="inlineStr">
+      <c r="E23" s="7" t="inlineStr">
         <is>
           <t>10-49</t>
         </is>
       </c>
-      <c r="F26" s="7" t="inlineStr">
+      <c r="F23" s="7" t="inlineStr">
         <is>
           <t>hatchstaff.com</t>
         </is>
       </c>
-      <c r="G26" s="7" t="n"/>
-      <c r="H26" s="7" t="inlineStr">
+      <c r="G23" s="7" t="n"/>
+      <c r="H23" s="7" t="inlineStr">
         <is>
           <t>Hatch</t>
         </is>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I23" s="7" t="n">
         <v>9000</v>
       </c>
-      <c r="J26" s="7" t="inlineStr">
+      <c r="J23" s="7" t="inlineStr">
         <is>
           <t>hatchstaff.com</t>
         </is>
       </c>
-      <c r="K26" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L26" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M26" s="9" t="n">
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M23" s="9" t="n">
         <v>75</v>
       </c>
-      <c r="N26" s="10" t="inlineStr">
+      <c r="N23" s="10" t="inlineStr">
         <is>
           <t>⚠️ ZI_Company_Name__c 'Hatch' does not match email domain 'hatchstaff.com'.
 ✅ ZI_Employees__c (9000) aligns with 'Enterprise' segment size range (10-49).
-✅ ZI_Company_Name__c 'Hatch' is consistent with SegmentName 'Enterprise'.</t>
-        </is>
-      </c>
-      <c r="O26" s="10" t="inlineStr">
+✅ ZI_Website__c missing; inferred as 'hatchstaff.com' based on email domain.</t>
+        </is>
+      </c>
+      <c r="O23" s="10" t="inlineStr">
         <is>
           <t>{
   "ZI_Company_Name__c": "Hatch Staffing Services"
 }</t>
         </is>
       </c>
-      <c r="P26" s="10" t="inlineStr"/>
-      <c r="Q26" s="7" t="inlineStr">
+      <c r="P23" s="10" t="inlineStr"/>
+      <c r="Q23" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="25" customHeight="1">
-      <c r="A27" s="7" t="inlineStr">
+    <row r="24" ht="25" customHeight="1">
+      <c r="A24" s="7" t="inlineStr">
         <is>
           <t>00Q2H00002Bmc54UAB</t>
         </is>
       </c>
-      <c r="B27" s="7" t="inlineStr">
+      <c r="B24" s="7" t="inlineStr">
         <is>
           <t>ksteinhoff@hbscu.com</t>
         </is>
       </c>
-      <c r="C27" s="7" t="inlineStr">
+      <c r="C24" s="7" t="inlineStr">
         <is>
           <t>List Purchase</t>
         </is>
       </c>
-      <c r="D27" s="7" t="inlineStr">
+      <c r="D24" s="7" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E27" s="7" t="n"/>
-      <c r="F27" s="7" t="inlineStr">
+      <c r="E24" s="7" t="n"/>
+      <c r="F24" s="7" t="inlineStr">
         <is>
           <t>heartlandbusinessservices.com</t>
         </is>
       </c>
-      <c r="G27" s="7" t="n"/>
-      <c r="H27" s="7" t="inlineStr">
+      <c r="G24" s="7" t="n"/>
+      <c r="H24" s="7" t="inlineStr">
         <is>
           <t>H&amp;R Block</t>
         </is>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I24" s="7" t="n">
         <v>46700</v>
       </c>
-      <c r="J27" s="7" t="inlineStr">
+      <c r="J24" s="7" t="inlineStr">
         <is>
           <t>hbscu.com</t>
         </is>
       </c>
-      <c r="K27" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L27" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M27" s="9" t="n">
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M24" s="9" t="n">
         <v>75</v>
       </c>
-      <c r="N27" s="10" t="inlineStr">
-        <is>
-          <t>⚠️ ZI_Company_Name__c 'H&amp;R Block' conflicts with email domain 'hbscu.com'.
-✅ ZI_Employees__c aligns with 'Enterprise' segment size range.
-✅ Email domain 'hbscu.com' matches Website 'heartlandbusinessservices.com'.</t>
-        </is>
-      </c>
-      <c r="O27" s="10" t="inlineStr">
+      <c r="N24" s="10" t="inlineStr">
+        <is>
+          <t>⚠️ ZI_Company_Name__c 'H&amp;R Block' does not match email domain 'hbscu.com'.
+✅ ZI_Employees__c (46700) aligns with 'Enterprise' segment size.
+✅ Corporate email domain 'hbscu.com' matches ZI_Company_Name__c 'H&amp;R Block'.</t>
+        </is>
+      </c>
+      <c r="O24" s="10" t="inlineStr">
         <is>
           <t>{
   "ZI_Company_Name__c": "Heartland Business Services"
 }</t>
         </is>
       </c>
-      <c r="P27" s="10" t="inlineStr"/>
-      <c r="Q27" s="7" t="inlineStr">
+      <c r="P24" s="10" t="inlineStr"/>
+      <c r="Q24" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="25" customHeight="1">
-      <c r="A28" s="7" t="inlineStr">
+    <row r="25" ht="25" customHeight="1">
+      <c r="A25" s="7" t="inlineStr">
         <is>
           <t>00Q2H00002BmcV7UAJ</t>
         </is>
       </c>
-      <c r="B28" s="7" t="inlineStr">
+      <c r="B25" s="7" t="inlineStr">
         <is>
           <t>mike.volynski@infoprosystems.net</t>
         </is>
       </c>
-      <c r="C28" s="7" t="inlineStr">
+      <c r="C25" s="7" t="inlineStr">
         <is>
           <t>List Purchase</t>
         </is>
       </c>
-      <c r="D28" s="7" t="inlineStr">
+      <c r="D25" s="7" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E28" s="7" t="n"/>
-      <c r="F28" s="7" t="inlineStr">
+      <c r="E25" s="7" t="n"/>
+      <c r="F25" s="7" t="inlineStr">
         <is>
           <t>infoprosystems.net</t>
         </is>
       </c>
-      <c r="G28" s="7" t="n"/>
-      <c r="H28" s="7" t="inlineStr">
+      <c r="G25" s="7" t="n"/>
+      <c r="H25" s="7" t="inlineStr">
         <is>
           <t>InfoPro Systems Inc</t>
         </is>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I25" s="7" t="n">
         <v>75612</v>
       </c>
-      <c r="J28" s="7" t="inlineStr">
+      <c r="J25" s="7" t="inlineStr">
         <is>
           <t>infoprosystems.net</t>
         </is>
       </c>
-      <c r="K28" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L28" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M28" s="9" t="n">
+      <c r="K25" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L25" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M25" s="9" t="n">
         <v>75</v>
       </c>
-      <c r="N28" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain and Website.
-✅ ZI_Employees__c aligns with Enterprise segment size.
-⚠️ LS_Company_Size_Range__c missing, could provide additional context.
-⚠️ Website missing in ZI_Website__c, inferred from email domain.
-⚠️ Large-company completeness check: ZI_Website__c is not populated.</t>
-        </is>
-      </c>
-      <c r="O28" s="10" t="inlineStr"/>
-      <c r="P28" s="10" t="inlineStr"/>
-      <c r="Q28" s="7" t="inlineStr">
+      <c r="N25" s="10" t="inlineStr">
+        <is>
+          <t>✅ ZI_Company_Name__c matches email domain and trusted internal data.
+✅ ZI_Employees__c aligns with the Enterprise segment size.
+⚠️ Website missing in enrichment; inferred primary site from trusted internal data.
+⚠️ Large-company completeness check: employee count present but website missing.</t>
+        </is>
+      </c>
+      <c r="O25" s="10" t="inlineStr"/>
+      <c r="P25" s="10" t="inlineStr"/>
+      <c r="Q25" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="25" customHeight="1">
-      <c r="A29" s="7" t="inlineStr">
+    <row r="26" ht="25" customHeight="1">
+      <c r="A26" s="7" t="inlineStr">
         <is>
           <t>00Q2H00002BmcWjUAJ</t>
         </is>
       </c>
-      <c r="B29" s="7" t="inlineStr">
+      <c r="B26" s="7" t="inlineStr">
         <is>
           <t>ochoa_felipe_x@solarturbines.com</t>
         </is>
       </c>
-      <c r="C29" s="7" t="inlineStr">
+      <c r="C26" s="7" t="inlineStr">
         <is>
           <t>List Purchase</t>
         </is>
       </c>
-      <c r="D29" s="7" t="inlineStr">
+      <c r="D26" s="7" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E29" s="7" t="inlineStr">
+      <c r="E26" s="7" t="inlineStr">
         <is>
           <t>1000+</t>
         </is>
       </c>
-      <c r="F29" s="7" t="inlineStr">
+      <c r="F26" s="7" t="inlineStr">
         <is>
           <t>www.caterpillar.com</t>
         </is>
       </c>
-      <c r="G29" s="7" t="n"/>
-      <c r="H29" s="7" t="inlineStr">
+      <c r="G26" s="7" t="n"/>
+      <c r="H26" s="7" t="inlineStr">
         <is>
           <t>Solar Turbines</t>
         </is>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I26" s="7" t="n">
         <v>8000</v>
       </c>
-      <c r="J29" s="7" t="inlineStr">
+      <c r="J26" s="7" t="inlineStr">
         <is>
           <t>solarturbines.com</t>
         </is>
       </c>
-      <c r="K29" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L29" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M29" s="11" t="n">
+      <c r="K26" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L26" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M26" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="N29" s="10" t="inlineStr">
+      <c r="N26" s="10" t="inlineStr">
         <is>
           <t>✅ ZI_Company_Name__c matches email domain and SegmentName 'Enterprise'.
 ✅ ZI_Employees__c (8000) aligns with LS_Company_Size_Range__c (1000+).
-⚠️ Website inconsistency: ZI_Website__c missing, should match Website 'www.caterpillar.com'.</t>
-        </is>
-      </c>
-      <c r="O29" s="10" t="inlineStr"/>
-      <c r="P29" s="10" t="inlineStr"/>
-      <c r="Q29" s="7" t="inlineStr">
+✅ Lead data consistent with ZoomInfo enrichment; no quality flags raised.</t>
+        </is>
+      </c>
+      <c r="O26" s="10" t="inlineStr"/>
+      <c r="P26" s="10" t="inlineStr"/>
+      <c r="Q26" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="25" customHeight="1">
-      <c r="A30" s="7" t="inlineStr">
+    <row r="27" ht="25" customHeight="1">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>00Q2H00002BmcxpUAB</t>
         </is>
       </c>
-      <c r="B30" s="7" t="inlineStr">
+      <c r="B27" s="7" t="inlineStr">
         <is>
           <t>rhoda.tamakloe@kaplanedfoundation.org</t>
         </is>
       </c>
-      <c r="C30" s="7" t="inlineStr">
+      <c r="C27" s="7" t="inlineStr">
         <is>
           <t>List Purchase</t>
         </is>
       </c>
-      <c r="D30" s="7" t="inlineStr">
+      <c r="D27" s="7" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E30" s="7" t="inlineStr">
+      <c r="E27" s="7" t="inlineStr">
         <is>
           <t>5000+</t>
         </is>
       </c>
-      <c r="F30" s="7" t="inlineStr">
+      <c r="F27" s="7" t="inlineStr">
         <is>
           <t>www.kaplan.com</t>
         </is>
       </c>
-      <c r="G30" s="7" t="n"/>
-      <c r="H30" s="7" t="inlineStr">
+      <c r="G27" s="7" t="n"/>
+      <c r="H27" s="7" t="inlineStr">
         <is>
           <t>Kaplan</t>
         </is>
       </c>
-      <c r="I30" s="7" t="n">
+      <c r="I27" s="7" t="n">
         <v>11900</v>
       </c>
-      <c r="J30" s="7" t="inlineStr">
+      <c r="J27" s="7" t="inlineStr">
         <is>
           <t>kaplanedfoundation.org</t>
         </is>
       </c>
-      <c r="K30" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L30" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M30" s="11" t="n">
+      <c r="K27" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L27" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M27" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="N30" s="10" t="inlineStr">
+      <c r="N27" s="10" t="inlineStr">
         <is>
           <t>✅ ZI_Company_Name__c matches email domain and trusted internal data.
 ✅ ZI_Employees__c aligns with LS_Company_Size_Range__c for a large enterprise.
 ⚠️ ZI_Website__c missing; inferred as 'kaplan.com' based on email domain.
-✅ No flags raised for incomplete or suspicious enrichment.</t>
+✅ No flags raised for incomplete enrichment or suspicious data.</t>
+        </is>
+      </c>
+      <c r="O27" s="10" t="inlineStr"/>
+      <c r="P27" s="10" t="inlineStr"/>
+      <c r="Q27" s="7" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="25" customHeight="1">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>00Q2H00002Bmd5kUAB</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>elissa@legacyadvisor.net</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
+          <t>List Purchase</t>
+        </is>
+      </c>
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="n"/>
+      <c r="F28" s="7" t="inlineStr">
+        <is>
+          <t>legacyadvisor.net</t>
+        </is>
+      </c>
+      <c r="G28" s="7" t="inlineStr">
+        <is>
+          <t>ameriprise.com</t>
+        </is>
+      </c>
+      <c r="H28" s="7" t="inlineStr">
+        <is>
+          <t>Ameriprise Financial</t>
+        </is>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>12374</v>
+      </c>
+      <c r="J28" s="7" t="inlineStr">
+        <is>
+          <t>legacyadvisor.net</t>
+        </is>
+      </c>
+      <c r="K28" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L28" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M28" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="N28" s="10" t="inlineStr">
+        <is>
+          <t>⚠️ ZI_Website__c (ameriprise.com) does not match lead's email domain (legacyadvisor.net).
+✅ ZI_Company_Name__c (Ameriprise Financial) aligns with ZI_Employees__c count (large company).</t>
+        </is>
+      </c>
+      <c r="O28" s="10" t="inlineStr"/>
+      <c r="P28" s="10" t="inlineStr">
+        <is>
+          <t>{
+  "ZI_Company_Name__c": "Legacy Advisor"
+}</t>
+        </is>
+      </c>
+      <c r="Q28" s="7" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="25" customHeight="1">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>00Q2H00002Bmh1IUAR</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>jshields@shieldslegal.com</t>
+        </is>
+      </c>
+      <c r="C29" s="7" t="inlineStr">
+        <is>
+          <t>List Purchase</t>
+        </is>
+      </c>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="n"/>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>shieldslegalgroup.com</t>
+        </is>
+      </c>
+      <c r="G29" s="7" t="n"/>
+      <c r="H29" s="7" t="inlineStr">
+        <is>
+          <t>Microsoft</t>
+        </is>
+      </c>
+      <c r="I29" s="7" t="n">
+        <v>210842</v>
+      </c>
+      <c r="J29" s="7" t="inlineStr">
+        <is>
+          <t>shieldslegal.com</t>
+        </is>
+      </c>
+      <c r="K29" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L29" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M29" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="N29" s="10" t="inlineStr">
+        <is>
+          <t>❌ ZI_Company_Name__c 'Microsoft' conflicts with email domain 'shieldslegal.com'.
+⚠️ Employee count '210,842' significantly differs from expected range for 'Enterprise' segment.</t>
+        </is>
+      </c>
+      <c r="O29" s="10" t="inlineStr">
+        <is>
+          <t>{
+  "ZI_Company_Name__c": "Shields Legal Group"
+}</t>
+        </is>
+      </c>
+      <c r="P29" s="10" t="inlineStr">
+        <is>
+          <t>{
+  "ZI_Employees__c": "Large company (&gt;= 100 employees)"
+}</t>
+        </is>
+      </c>
+      <c r="Q29" s="7" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="25" customHeight="1">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>00Q2H00002BmhD6UAJ</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="inlineStr">
+        <is>
+          <t>skbennington@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C30" s="7" t="inlineStr">
+        <is>
+          <t>Affiliates</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>1000+</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="n"/>
+      <c r="G30" s="7" t="n"/>
+      <c r="H30" s="7" t="inlineStr">
+        <is>
+          <t>H&amp;R Block</t>
+        </is>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>46700</v>
+      </c>
+      <c r="J30" s="7" t="inlineStr">
+        <is>
+          <t>yahoo.com</t>
+        </is>
+      </c>
+      <c r="K30" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L30" s="12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M30" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="N30" s="10" t="inlineStr">
+        <is>
+          <t>❌  Suspicious enrichment flag raised due to free email domain and missing website.
+⚠️  Major discrepancy in employee count (46700) for Enterprise segment (1000+ range).</t>
         </is>
       </c>
       <c r="O30" s="10" t="inlineStr"/>

</xml_diff>

<commit_message>
data types added to each lead field for better mapping
</commit_message>
<xml_diff>
--- a/docs/sample_result.xlsx
+++ b/docs/sample_result.xlsx
@@ -544,7 +544,7 @@
     <row r="2" ht="25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2025-07-02 13:09:53</t>
+          <t>Generated: 2025-07-03 09:18:31</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>65.5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
@@ -676,7 +676,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>27.51s</t>
+          <t>35.27s</t>
         </is>
       </c>
     </row>
@@ -829,9 +829,10 @@
       </c>
       <c r="N21" s="10" t="inlineStr">
         <is>
-          <t>✅ ZI_Company_Name__c matches email domain; strong brand alignment.
-⚠️ ZI_Website__c is missing; inferred primary site from email domain.
-✅ ZI_Employees__c consistent with Enterprise segment size range.</t>
+          <t>✅ ZI_Company_Name__c matches email domain; high brand consistency.
+✅ ZI_Employees__c aligns with LS_Company_Size_Range__c; no major discrepancy.
+⚠️ ZI_Website__c missing; inferred primary site from email domain.
+⚠️ Large-company completeness check: website missing despite high employee count.</t>
         </is>
       </c>
       <c r="O21" s="10" t="inlineStr"/>
@@ -898,8 +899,9 @@
       </c>
       <c r="N22" s="10" t="inlineStr">
         <is>
-          <t>⚠️ ZI_Company_Name__c 'Medtronic' conflicts with email domain 'emilydavisconsulting.com'.
-✅ ZI_Employees__c aligns with 'Enterprise' segment size; no size-range conflict.</t>
+          <t>⚠️ ZI_Company_Name__c 'Medtronic' does not match email domain 'emilydavisconsulting.com'.
+✅ ZI_Employees__c aligns with 'Enterprise' segment size expectations.
+⚠️ Website missing in ZoomInfo enrichment; inferred primary site from email domain.</t>
         </is>
       </c>
       <c r="O22" s="10" t="inlineStr">
@@ -976,18 +978,12 @@
       </c>
       <c r="N23" s="10" t="inlineStr">
         <is>
-          <t>⚠️ ZI_Company_Name__c 'Hatch' does not match email domain 'hatchstaff.com'.
-✅ ZI_Employees__c (9000) aligns with 'Enterprise' segment size range (10-49).
-✅ ZI_Website__c missing; inferred as 'hatchstaff.com' based on email domain.</t>
-        </is>
-      </c>
-      <c r="O23" s="10" t="inlineStr">
-        <is>
-          <t>{
-  "ZI_Company_Name__c": "Hatch Staffing Services"
-}</t>
-        </is>
-      </c>
+          <t>✅ ZI_Employees__c consistent with Enterprise segment size range.
+⚠️ Website field blank; inferred primary site from ZoomInfo enrichment.
+✅ ZI_Company_Name__c aligns with email domain, strengthening company match.</t>
+        </is>
+      </c>
+      <c r="O23" s="10" t="inlineStr"/>
       <c r="P23" s="10" t="inlineStr"/>
       <c r="Q23" s="7" t="inlineStr">
         <is>
@@ -1051,9 +1047,8 @@
       </c>
       <c r="N24" s="10" t="inlineStr">
         <is>
-          <t>⚠️ ZI_Company_Name__c 'H&amp;R Block' does not match email domain 'hbscu.com'.
-✅ ZI_Employees__c (46700) aligns with 'Enterprise' segment size.
-✅ Corporate email domain 'hbscu.com' matches ZI_Company_Name__c 'H&amp;R Block'.</t>
+          <t>✅ ZI_Employees__c aligns with Enterprise segment size; no major discrepancy.
+⚠️ Website field blank; inferred primary site from ZoomInfo enrichment.</t>
         </is>
       </c>
       <c r="O24" s="10" t="inlineStr">
@@ -1195,14 +1190,14 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M26" s="6" t="n">
-        <v>90</v>
+      <c r="M26" s="9" t="n">
+        <v>75</v>
       </c>
       <c r="N26" s="10" t="inlineStr">
         <is>
           <t>✅ ZI_Company_Name__c matches email domain and SegmentName 'Enterprise'.
-✅ ZI_Employees__c (8000) aligns with LS_Company_Size_Range__c (1000+).
-✅ Lead data consistent with ZoomInfo enrichment; no quality flags raised.</t>
+✅ ZI_Employees__c aligns with LS_Company_Size_Range__c '1000+'.
+⚠️ Website inconsistency: ZI_Website__c missing, should match Website 'www.caterpillar.com'.</t>
         </is>
       </c>
       <c r="O26" s="10" t="inlineStr"/>
@@ -1268,15 +1263,15 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M27" s="6" t="n">
-        <v>90</v>
+      <c r="M27" s="9" t="n">
+        <v>75</v>
       </c>
       <c r="N27" s="10" t="inlineStr">
         <is>
-          <t>✅ ZI_Company_Name__c matches email domain and trusted internal data.
-✅ ZI_Employees__c aligns with LS_Company_Size_Range__c for a large enterprise.
+          <t>✅ ZI_Company_Name__c matches email domain and Website.
+✅ ZI_Employees__c aligns with LS_Company_Size_Range__c for Enterprise segment.
 ⚠️ ZI_Website__c missing; inferred as 'kaplan.com' based on email domain.
-✅ No flags raised for incomplete enrichment or suspicious data.</t>
+⚠️ Large-company completeness check: ZI_Website__c is not populated.</t>
         </is>
       </c>
       <c r="O27" s="10" t="inlineStr"/>
@@ -1347,18 +1342,24 @@
       </c>
       <c r="N28" s="10" t="inlineStr">
         <is>
-          <t>⚠️ ZI_Website__c (ameriprise.com) does not match lead's email domain (legacyadvisor.net).
-✅ ZI_Company_Name__c (Ameriprise Financial) aligns with ZI_Employees__c count (large company).</t>
-        </is>
-      </c>
-      <c r="O28" s="10" t="inlineStr"/>
-      <c r="P28" s="10" t="inlineStr">
+          <t>⚠️ ZI_Website__c (ameriprise.com) and ZI_Company_Name__c (Ameriprise Financial) do not match lead's email domain (legacyadvisor.net).
+✅ ZI_Employees__c (12374) aligns with the Enterprise segment, but LS_Company_Size_Range__c is missing for comparison.</t>
+        </is>
+      </c>
+      <c r="O28" s="10" t="inlineStr">
         <is>
           <t>{
   "ZI_Company_Name__c": "Legacy Advisor"
 }</t>
         </is>
       </c>
+      <c r="P28" s="10" t="inlineStr">
+        <is>
+          <t>{
+  "ZI_Employees__c": 5000
+}</t>
+        </is>
+      </c>
       <c r="Q28" s="7" t="inlineStr">
         <is>
           <t>success</t>
@@ -1421,8 +1422,9 @@
       </c>
       <c r="N29" s="10" t="inlineStr">
         <is>
-          <t>❌ ZI_Company_Name__c 'Microsoft' conflicts with email domain 'shieldslegal.com'.
-⚠️ Employee count '210,842' significantly differs from expected range for 'Enterprise' segment.</t>
+          <t>❌ Company name 'Microsoft' conflicts with email domain 'shieldslegal.com'.
+⚠️ Employee count (210,842) significantly exceeds Enterprise segment size expectations.
+⚠️ Website inconsistency between lead-provided and enriched data.</t>
         </is>
       </c>
       <c r="O29" s="10" t="inlineStr">
@@ -1435,7 +1437,7 @@
       <c r="P29" s="10" t="inlineStr">
         <is>
           <t>{
-  "ZI_Employees__c": "Large company (&gt;= 100 employees)"
+  "ZI_Employees__c": "100-250"
 }</t>
         </is>
       </c>
@@ -1497,12 +1499,12 @@
         </is>
       </c>
       <c r="M30" s="11" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="N30" s="10" t="inlineStr">
         <is>
-          <t>❌  Suspicious enrichment flag raised due to free email domain and missing website.
-⚠️  Major discrepancy in employee count (46700) for Enterprise segment (1000+ range).</t>
+          <t>❌ Large discrepancy in employee count (46700) and LS_Company_Size_Range__c (1000+).
+⚠️ Lead has a free email domain (yahoo.com) but enriched company is H&amp;R Block, raising authenticity concerns.</t>
         </is>
       </c>
       <c r="O30" s="10" t="inlineStr"/>

</xml_diff>

<commit_message>
add company field + fixed excel export appending for excel inputs
</commit_message>
<xml_diff>
--- a/docs/sample_result.xlsx
+++ b/docs/sample_result.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,12 +41,8 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="002B2926"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -77,12 +73,6 @@
         <bgColor rgb="00DC3545"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFE6E6"/>
-        <bgColor rgb="00FFE6E6"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -110,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -137,9 +127,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,7 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,15 +510,16 @@
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="40" customWidth="1" min="14" max="14"/>
-    <col width="25" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="40" customWidth="1" min="15" max="15"/>
     <col width="25" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="25" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -544,7 +532,7 @@
     <row r="2" ht="25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2025-07-03 09:18:31</t>
+          <t>Generated: 2025-07-03 13:31:33</t>
         </is>
       </c>
     </row>
@@ -583,7 +571,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
@@ -594,7 +582,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -605,7 +593,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>65</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1">
@@ -625,7 +613,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="25" customHeight="1">
@@ -664,7 +652,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>SELECT Id FROM Lead WHERE ZI_Employees__c &gt; 2000</t>
+          <t>SELECT Id FROM Lead WHERE ZI_Employees__c &gt; 1000</t>
         </is>
       </c>
     </row>
@@ -676,7 +664,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>35.27s</t>
+          <t>25.35s</t>
         </is>
       </c>
     </row>
@@ -715,55 +703,60 @@
       </c>
       <c r="G20" s="6" t="inlineStr">
         <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="H20" s="6" t="inlineStr">
+        <is>
           <t>ZI Website</t>
         </is>
       </c>
-      <c r="H20" s="6" t="inlineStr">
+      <c r="I20" s="6" t="inlineStr">
         <is>
           <t>ZI Company Name</t>
         </is>
       </c>
-      <c r="I20" s="6" t="inlineStr">
+      <c r="J20" s="6" t="inlineStr">
         <is>
           <t>ZI Employees</t>
         </is>
       </c>
-      <c r="J20" s="6" t="inlineStr">
+      <c r="K20" s="6" t="inlineStr">
         <is>
           <t>Email Domain</t>
         </is>
       </c>
-      <c r="K20" s="6" t="inlineStr">
+      <c r="L20" s="6" t="inlineStr">
         <is>
           <t>Not in TAM</t>
         </is>
       </c>
-      <c r="L20" s="6" t="inlineStr">
+      <c r="M20" s="6" t="inlineStr">
         <is>
           <t>Suspicious Enrichment</t>
         </is>
       </c>
-      <c r="M20" s="6" t="inlineStr">
+      <c r="N20" s="6" t="inlineStr">
         <is>
           <t>Confidence Score</t>
         </is>
       </c>
-      <c r="N20" s="6" t="inlineStr">
+      <c r="O20" s="6" t="inlineStr">
         <is>
           <t>Explanation</t>
         </is>
       </c>
-      <c r="O20" s="6" t="inlineStr">
+      <c r="P20" s="6" t="inlineStr">
         <is>
           <t>Corrections</t>
         </is>
       </c>
-      <c r="P20" s="6" t="inlineStr">
+      <c r="Q20" s="6" t="inlineStr">
         <is>
           <t>Inferences</t>
         </is>
       </c>
-      <c r="Q20" s="6" t="inlineStr">
+      <c r="R20" s="6" t="inlineStr">
         <is>
           <t>AI Status</t>
         </is>
@@ -772,12 +765,12 @@
     <row r="21" ht="25" customHeight="1">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmaghUAB</t>
+          <t>00Q2H00002BmYXcUAN</t>
         </is>
       </c>
       <c r="B21" s="7" t="inlineStr">
         <is>
-          <t>david_edelman@edelman-lyon.com</t>
+          <t>skwiker@plymouthrock.com</t>
         </is>
       </c>
       <c r="C21" s="7" t="inlineStr">
@@ -787,36 +780,32 @@
       </c>
       <c r="D21" s="7" t="inlineStr">
         <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E21" s="7" t="inlineStr">
-        <is>
-          <t>400-4999</t>
-        </is>
-      </c>
+          <t>Majors</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="n"/>
       <c r="F21" s="7" t="inlineStr">
         <is>
-          <t>edelman.com</t>
-        </is>
-      </c>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="7" t="inlineStr">
-        <is>
-          <t>Daniel J Edelman Holdings Inc</t>
-        </is>
-      </c>
-      <c r="I21" s="7" t="n">
-        <v>5610</v>
-      </c>
-      <c r="J21" s="7" t="inlineStr">
-        <is>
-          <t>edelman-lyon.com</t>
-        </is>
-      </c>
-      <c r="K21" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>bunkerhillins.com</t>
+        </is>
+      </c>
+      <c r="G21" s="7" t="inlineStr">
+        <is>
+          <t>Bunker Hill Insurance Company</t>
+        </is>
+      </c>
+      <c r="H21" s="7" t="n"/>
+      <c r="I21" s="7" t="inlineStr">
+        <is>
+          <t>Bunker Hill</t>
+        </is>
+      </c>
+      <c r="J21" s="7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="K21" s="7" t="inlineStr">
+        <is>
+          <t>plymouthrock.com</t>
         </is>
       </c>
       <c r="L21" s="8" t="inlineStr">
@@ -824,20 +813,29 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M21" s="9" t="n">
+      <c r="M21" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N21" s="9" t="n">
         <v>75</v>
       </c>
-      <c r="N21" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain; high brand consistency.
-✅ ZI_Employees__c aligns with LS_Company_Size_Range__c; no major discrepancy.
-⚠️ ZI_Website__c missing; inferred primary site from email domain.
-⚠️ Large-company completeness check: website missing despite high employee count.</t>
-        </is>
-      </c>
-      <c r="O21" s="10" t="inlineStr"/>
+      <c r="O21" s="10" t="inlineStr">
+        <is>
+          <t>✅ ZI_Employees__c consistent with large company segment; no size-range conflict.
+⚠️ Website field blank; inferred primary site from ZoomInfo enrichment.</t>
+        </is>
+      </c>
       <c r="P21" s="10" t="inlineStr"/>
-      <c r="Q21" s="7" t="inlineStr">
+      <c r="Q21" s="10" t="inlineStr">
+        <is>
+          <t>{
+  "ZI_Company_Name__c": "Plymouth Rock"
+}</t>
+        </is>
+      </c>
+      <c r="R21" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -846,12 +844,12 @@
     <row r="22" ht="25" customHeight="1">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmapUUAR</t>
+          <t>00Q2H00002BmYn2UAF</t>
         </is>
       </c>
       <c r="B22" s="7" t="inlineStr">
         <is>
-          <t>emily@emilydavisconsulting.com</t>
+          <t>michael.strouch@cedarpointfinancial.com</t>
         </is>
       </c>
       <c r="C22" s="7" t="inlineStr">
@@ -861,32 +859,32 @@
       </c>
       <c r="D22" s="7" t="inlineStr">
         <is>
-          <t>Enterprise</t>
+          <t>Majors</t>
         </is>
       </c>
       <c r="E22" s="7" t="n"/>
       <c r="F22" s="7" t="inlineStr">
         <is>
-          <t>emilydavisconsulting.com</t>
-        </is>
-      </c>
-      <c r="G22" s="7" t="n"/>
-      <c r="H22" s="7" t="inlineStr">
-        <is>
-          <t>Medtronic</t>
-        </is>
-      </c>
-      <c r="I22" s="7" t="n">
-        <v>95000</v>
-      </c>
-      <c r="J22" s="7" t="inlineStr">
-        <is>
-          <t>emilydavisconsulting.com</t>
-        </is>
-      </c>
-      <c r="K22" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>cedarpointfinancial.com</t>
+        </is>
+      </c>
+      <c r="G22" s="7" t="inlineStr">
+        <is>
+          <t>Cedar Point Financial Services LLC</t>
+        </is>
+      </c>
+      <c r="H22" s="7" t="n"/>
+      <c r="I22" s="7" t="inlineStr">
+        <is>
+          <t>Fairfield University</t>
+        </is>
+      </c>
+      <c r="J22" s="7" t="n">
+        <v>1477</v>
+      </c>
+      <c r="K22" s="7" t="inlineStr">
+        <is>
+          <t>cedarpointfinancial.com</t>
         </is>
       </c>
       <c r="L22" s="8" t="inlineStr">
@@ -894,25 +892,24 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M22" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="N22" s="10" t="inlineStr">
-        <is>
-          <t>⚠️ ZI_Company_Name__c 'Medtronic' does not match email domain 'emilydavisconsulting.com'.
-✅ ZI_Employees__c aligns with 'Enterprise' segment size expectations.
-⚠️ Website missing in ZoomInfo enrichment; inferred primary site from email domain.</t>
-        </is>
+      <c r="M22" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N22" s="9" t="n">
+        <v>75</v>
       </c>
       <c r="O22" s="10" t="inlineStr">
         <is>
-          <t>{
-  "ZI_Company_Name__c": "Emily Davis Consulting"
-}</t>
+          <t>⚠️ ZI_Company_Name__c 'Fairfield University' does not match lead's Company 'Cedar Point Financial Services LLC'.
+✅ ZI_Employees__c (1477) aligns with the lead's SegmentName 'Majors'.
+✅ Email domain, website, and company are consistent.</t>
         </is>
       </c>
       <c r="P22" s="10" t="inlineStr"/>
-      <c r="Q22" s="7" t="inlineStr">
+      <c r="Q22" s="10" t="inlineStr"/>
+      <c r="R22" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -921,12 +918,12 @@
     <row r="23" ht="25" customHeight="1">
       <c r="A23" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmblPUAR</t>
+          <t>00Q2H00002BmYvVUAV</t>
         </is>
       </c>
       <c r="B23" s="7" t="inlineStr">
         <is>
-          <t>lori@hatchstaff.com</t>
+          <t>scott.campbell@chicagofed.org</t>
         </is>
       </c>
       <c r="C23" s="7" t="inlineStr">
@@ -936,36 +933,36 @@
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>Enterprise</t>
+          <t>Majors</t>
         </is>
       </c>
       <c r="E23" s="7" t="inlineStr">
         <is>
-          <t>10-49</t>
+          <t>20-99</t>
         </is>
       </c>
       <c r="F23" s="7" t="inlineStr">
         <is>
-          <t>hatchstaff.com</t>
-        </is>
-      </c>
-      <c r="G23" s="7" t="n"/>
-      <c r="H23" s="7" t="inlineStr">
-        <is>
-          <t>Hatch</t>
-        </is>
-      </c>
-      <c r="I23" s="7" t="n">
-        <v>9000</v>
-      </c>
-      <c r="J23" s="7" t="inlineStr">
-        <is>
-          <t>hatchstaff.com</t>
-        </is>
-      </c>
-      <c r="K23" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>www.chicagofed.org</t>
+        </is>
+      </c>
+      <c r="G23" s="7" t="inlineStr">
+        <is>
+          <t>Federal Reserve Bank of Chicago</t>
+        </is>
+      </c>
+      <c r="H23" s="7" t="n"/>
+      <c r="I23" s="7" t="inlineStr">
+        <is>
+          <t>Federal Reserve Bank of Chicago</t>
+        </is>
+      </c>
+      <c r="J23" s="7" t="n">
+        <v>1580</v>
+      </c>
+      <c r="K23" s="7" t="inlineStr">
+        <is>
+          <t>chicagofed.org</t>
         </is>
       </c>
       <c r="L23" s="8" t="inlineStr">
@@ -973,19 +970,25 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M23" s="9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N23" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Employees__c consistent with Enterprise segment size range.
-⚠️ Website field blank; inferred primary site from ZoomInfo enrichment.
-✅ ZI_Company_Name__c aligns with email domain, strengthening company match.</t>
-        </is>
-      </c>
-      <c r="O23" s="10" t="inlineStr"/>
+      <c r="M23" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N23" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="O23" s="10" t="inlineStr">
+        <is>
+          <t>✅ ZI_Company_Name__c matches Company and email domain - strong consistency.
+✅ ZI_Employees__c aligns with large company segment and internal size range.
+⚠️ Website missing in ZoomInfo enrichment, inferred from trusted Website field.
+✅ No flags raised for incomplete or suspicious enrichment.</t>
+        </is>
+      </c>
       <c r="P23" s="10" t="inlineStr"/>
-      <c r="Q23" s="7" t="inlineStr">
+      <c r="Q23" s="10" t="inlineStr"/>
+      <c r="R23" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -994,12 +997,12 @@
     <row r="24" ht="25" customHeight="1">
       <c r="A24" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002Bmc54UAB</t>
+          <t>00Q2H00002BmaghUAB</t>
         </is>
       </c>
       <c r="B24" s="7" t="inlineStr">
         <is>
-          <t>ksteinhoff@hbscu.com</t>
+          <t>david_edelman@edelman-lyon.com</t>
         </is>
       </c>
       <c r="C24" s="7" t="inlineStr">
@@ -1012,29 +1015,33 @@
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E24" s="7" t="n"/>
+      <c r="E24" s="7" t="inlineStr">
+        <is>
+          <t>400-4999</t>
+        </is>
+      </c>
       <c r="F24" s="7" t="inlineStr">
         <is>
-          <t>heartlandbusinessservices.com</t>
-        </is>
-      </c>
-      <c r="G24" s="7" t="n"/>
-      <c r="H24" s="7" t="inlineStr">
-        <is>
-          <t>H&amp;R Block</t>
-        </is>
-      </c>
-      <c r="I24" s="7" t="n">
-        <v>46700</v>
-      </c>
-      <c r="J24" s="7" t="inlineStr">
-        <is>
-          <t>hbscu.com</t>
-        </is>
-      </c>
-      <c r="K24" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>edelman.com</t>
+        </is>
+      </c>
+      <c r="G24" s="7" t="inlineStr">
+        <is>
+          <t>Edelman Co</t>
+        </is>
+      </c>
+      <c r="H24" s="7" t="n"/>
+      <c r="I24" s="7" t="inlineStr">
+        <is>
+          <t>Daniel J Edelman Holdings Inc</t>
+        </is>
+      </c>
+      <c r="J24" s="7" t="n">
+        <v>5610</v>
+      </c>
+      <c r="K24" s="7" t="inlineStr">
+        <is>
+          <t>edelman-lyon.com</t>
         </is>
       </c>
       <c r="L24" s="8" t="inlineStr">
@@ -1042,24 +1049,30 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M24" s="9" t="n">
+      <c r="M24" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N24" s="9" t="n">
         <v>75</v>
       </c>
-      <c r="N24" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Employees__c aligns with Enterprise segment size; no major discrepancy.
-⚠️ Website field blank; inferred primary site from ZoomInfo enrichment.</t>
-        </is>
-      </c>
       <c r="O24" s="10" t="inlineStr">
         <is>
+          <t>⚠️ ZI_Company_Name__c does not match Company field (Edelman Co) or email domain.
+✅ ZI_Employees__c (5610) aligns with LS_Company_Size_Range__c (400-4999) for Enterprise segment.
+⚠️ Website and ZI_Website__c are missing; inferred primary site from email domain.</t>
+        </is>
+      </c>
+      <c r="P24" s="10" t="inlineStr"/>
+      <c r="Q24" s="10" t="inlineStr">
+        <is>
           <t>{
-  "ZI_Company_Name__c": "Heartland Business Services"
+  "ZI_Website__c": "edelman-lyon.com"
 }</t>
         </is>
       </c>
-      <c r="P24" s="10" t="inlineStr"/>
-      <c r="Q24" s="7" t="inlineStr">
+      <c r="R24" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1068,12 +1081,12 @@
     <row r="25" ht="25" customHeight="1">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmcV7UAJ</t>
+          <t>00Q2H00002BmapUUAR</t>
         </is>
       </c>
       <c r="B25" s="7" t="inlineStr">
         <is>
-          <t>mike.volynski@infoprosystems.net</t>
+          <t>emily@emilydavisconsulting.com</t>
         </is>
       </c>
       <c r="C25" s="7" t="inlineStr">
@@ -1089,26 +1102,26 @@
       <c r="E25" s="7" t="n"/>
       <c r="F25" s="7" t="inlineStr">
         <is>
-          <t>infoprosystems.net</t>
-        </is>
-      </c>
-      <c r="G25" s="7" t="n"/>
-      <c r="H25" s="7" t="inlineStr">
-        <is>
-          <t>InfoPro Systems Inc</t>
-        </is>
-      </c>
-      <c r="I25" s="7" t="n">
-        <v>75612</v>
-      </c>
-      <c r="J25" s="7" t="inlineStr">
-        <is>
-          <t>infoprosystems.net</t>
-        </is>
-      </c>
-      <c r="K25" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>emilydavisconsulting.com</t>
+        </is>
+      </c>
+      <c r="G25" s="7" t="inlineStr">
+        <is>
+          <t>Emily Davis Consulting</t>
+        </is>
+      </c>
+      <c r="H25" s="7" t="n"/>
+      <c r="I25" s="7" t="inlineStr">
+        <is>
+          <t>Medtronic</t>
+        </is>
+      </c>
+      <c r="J25" s="7" t="n">
+        <v>95000</v>
+      </c>
+      <c r="K25" s="7" t="inlineStr">
+        <is>
+          <t>emilydavisconsulting.com</t>
         </is>
       </c>
       <c r="L25" s="8" t="inlineStr">
@@ -1116,20 +1129,23 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M25" s="9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N25" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain and trusted internal data.
-✅ ZI_Employees__c aligns with the Enterprise segment size.
-⚠️ Website missing in enrichment; inferred primary site from trusted internal data.
-⚠️ Large-company completeness check: employee count present but website missing.</t>
-        </is>
-      </c>
-      <c r="O25" s="10" t="inlineStr"/>
+      <c r="M25" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N25" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="O25" s="10" t="inlineStr">
+        <is>
+          <t>❌ ZI_Company_Name__c 'Medtronic' conflicts with lead Company 'Emily Davis Consulting'.
+⚠️ ZI_Employees__c (95,000) significantly higher than expected for 'Enterprise' segment.</t>
+        </is>
+      </c>
       <c r="P25" s="10" t="inlineStr"/>
-      <c r="Q25" s="7" t="inlineStr">
+      <c r="Q25" s="10" t="inlineStr"/>
+      <c r="R25" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1138,12 +1154,12 @@
     <row r="26" ht="25" customHeight="1">
       <c r="A26" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmcWjUAJ</t>
+          <t>00Q2H00002BmblPUAR</t>
         </is>
       </c>
       <c r="B26" s="7" t="inlineStr">
         <is>
-          <t>ochoa_felipe_x@solarturbines.com</t>
+          <t>lori@hatchstaff.com</t>
         </is>
       </c>
       <c r="C26" s="7" t="inlineStr">
@@ -1158,31 +1174,31 @@
       </c>
       <c r="E26" s="7" t="inlineStr">
         <is>
-          <t>1000+</t>
+          <t>10-49</t>
         </is>
       </c>
       <c r="F26" s="7" t="inlineStr">
         <is>
-          <t>www.caterpillar.com</t>
-        </is>
-      </c>
-      <c r="G26" s="7" t="n"/>
-      <c r="H26" s="7" t="inlineStr">
-        <is>
-          <t>Solar Turbines</t>
-        </is>
-      </c>
-      <c r="I26" s="7" t="n">
-        <v>8000</v>
-      </c>
-      <c r="J26" s="7" t="inlineStr">
-        <is>
-          <t>solarturbines.com</t>
-        </is>
-      </c>
-      <c r="K26" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>hatchstaff.com</t>
+        </is>
+      </c>
+      <c r="G26" s="7" t="inlineStr">
+        <is>
+          <t>Hatch Staffing Services</t>
+        </is>
+      </c>
+      <c r="H26" s="7" t="n"/>
+      <c r="I26" s="7" t="inlineStr">
+        <is>
+          <t>Hatch</t>
+        </is>
+      </c>
+      <c r="J26" s="7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="K26" s="7" t="inlineStr">
+        <is>
+          <t>hatchstaff.com</t>
         </is>
       </c>
       <c r="L26" s="8" t="inlineStr">
@@ -1190,19 +1206,24 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M26" s="9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N26" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain and SegmentName 'Enterprise'.
-✅ ZI_Employees__c aligns with LS_Company_Size_Range__c '1000+'.
-⚠️ Website inconsistency: ZI_Website__c missing, should match Website 'www.caterpillar.com'.</t>
-        </is>
-      </c>
-      <c r="O26" s="10" t="inlineStr"/>
+      <c r="M26" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N26" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="O26" s="10" t="inlineStr">
+        <is>
+          <t>⚠️ ZI_Website__c and ZI_Company_Name__c are missing, impacting completeness.
+✅ ZI_Employees__c aligns with Enterprise segment size range.
+⚠️ Website and Company name consistency with ZoomInfo enrichment needs validation.</t>
+        </is>
+      </c>
       <c r="P26" s="10" t="inlineStr"/>
-      <c r="Q26" s="7" t="inlineStr">
+      <c r="Q26" s="10" t="inlineStr"/>
+      <c r="R26" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1211,12 +1232,12 @@
     <row r="27" ht="25" customHeight="1">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmcxpUAB</t>
+          <t>00Q2H00002Bmc54UAB</t>
         </is>
       </c>
       <c r="B27" s="7" t="inlineStr">
         <is>
-          <t>rhoda.tamakloe@kaplanedfoundation.org</t>
+          <t>ksteinhoff@hbscu.com</t>
         </is>
       </c>
       <c r="C27" s="7" t="inlineStr">
@@ -1229,33 +1250,29 @@
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E27" s="7" t="inlineStr">
-        <is>
-          <t>5000+</t>
-        </is>
-      </c>
+      <c r="E27" s="7" t="n"/>
       <c r="F27" s="7" t="inlineStr">
         <is>
-          <t>www.kaplan.com</t>
-        </is>
-      </c>
-      <c r="G27" s="7" t="n"/>
-      <c r="H27" s="7" t="inlineStr">
-        <is>
-          <t>Kaplan</t>
-        </is>
-      </c>
-      <c r="I27" s="7" t="n">
-        <v>11900</v>
-      </c>
-      <c r="J27" s="7" t="inlineStr">
-        <is>
-          <t>kaplanedfoundation.org</t>
-        </is>
-      </c>
-      <c r="K27" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>heartlandbusinessservices.com</t>
+        </is>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>Heartland Business Services</t>
+        </is>
+      </c>
+      <c r="H27" s="7" t="n"/>
+      <c r="I27" s="7" t="inlineStr">
+        <is>
+          <t>H&amp;R Block</t>
+        </is>
+      </c>
+      <c r="J27" s="7" t="n">
+        <v>46700</v>
+      </c>
+      <c r="K27" s="7" t="inlineStr">
+        <is>
+          <t>hbscu.com</t>
         </is>
       </c>
       <c r="L27" s="8" t="inlineStr">
@@ -1263,20 +1280,24 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M27" s="9" t="n">
-        <v>75</v>
-      </c>
-      <c r="N27" s="10" t="inlineStr">
-        <is>
-          <t>✅ ZI_Company_Name__c matches email domain and Website.
-✅ ZI_Employees__c aligns with LS_Company_Size_Range__c for Enterprise segment.
-⚠️ ZI_Website__c missing; inferred as 'kaplan.com' based on email domain.
-⚠️ Large-company completeness check: ZI_Website__c is not populated.</t>
-        </is>
-      </c>
-      <c r="O27" s="10" t="inlineStr"/>
+      <c r="M27" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N27" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="O27" s="10" t="inlineStr">
+        <is>
+          <t>⚠️ ZI_Company_Name__c 'H&amp;R Block' does not match lead Company 'Heartland Business Services'.
+✅ ZI_Employees__c aligns with Enterprise segment size; no major discrepancy.
+⚠️ Website missing in ZoomInfo enrichment; inferred primary site from lead data.</t>
+        </is>
+      </c>
       <c r="P27" s="10" t="inlineStr"/>
-      <c r="Q27" s="7" t="inlineStr">
+      <c r="Q27" s="10" t="inlineStr"/>
+      <c r="R27" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1285,12 +1306,12 @@
     <row r="28" ht="25" customHeight="1">
       <c r="A28" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002Bmd5kUAB</t>
+          <t>00Q2H00002BmcV7UAJ</t>
         </is>
       </c>
       <c r="B28" s="7" t="inlineStr">
         <is>
-          <t>elissa@legacyadvisor.net</t>
+          <t>mike.volynski@infoprosystems.net</t>
         </is>
       </c>
       <c r="C28" s="7" t="inlineStr">
@@ -1306,30 +1327,26 @@
       <c r="E28" s="7" t="n"/>
       <c r="F28" s="7" t="inlineStr">
         <is>
-          <t>legacyadvisor.net</t>
+          <t>infoprosystems.net</t>
         </is>
       </c>
       <c r="G28" s="7" t="inlineStr">
         <is>
-          <t>ameriprise.com</t>
-        </is>
-      </c>
-      <c r="H28" s="7" t="inlineStr">
-        <is>
-          <t>Ameriprise Financial</t>
-        </is>
-      </c>
-      <c r="I28" s="7" t="n">
-        <v>12374</v>
-      </c>
-      <c r="J28" s="7" t="inlineStr">
-        <is>
-          <t>legacyadvisor.net</t>
-        </is>
-      </c>
-      <c r="K28" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>InfoPro Systems, Inc.</t>
+        </is>
+      </c>
+      <c r="H28" s="7" t="n"/>
+      <c r="I28" s="7" t="inlineStr">
+        <is>
+          <t>InfoPro Systems Inc</t>
+        </is>
+      </c>
+      <c r="J28" s="7" t="n">
+        <v>75612</v>
+      </c>
+      <c r="K28" s="7" t="inlineStr">
+        <is>
+          <t>infoprosystems.net</t>
         </is>
       </c>
       <c r="L28" s="8" t="inlineStr">
@@ -1337,30 +1354,25 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M28" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="N28" s="10" t="inlineStr">
-        <is>
-          <t>⚠️ ZI_Website__c (ameriprise.com) and ZI_Company_Name__c (Ameriprise Financial) do not match lead's email domain (legacyadvisor.net).
-✅ ZI_Employees__c (12374) aligns with the Enterprise segment, but LS_Company_Size_Range__c is missing for comparison.</t>
-        </is>
+      <c r="M28" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N28" s="9" t="n">
+        <v>75</v>
       </c>
       <c r="O28" s="10" t="inlineStr">
         <is>
-          <t>{
-  "ZI_Company_Name__c": "Legacy Advisor"
-}</t>
-        </is>
-      </c>
-      <c r="P28" s="10" t="inlineStr">
-        <is>
-          <t>{
-  "ZI_Employees__c": 5000
-}</t>
-        </is>
-      </c>
-      <c r="Q28" s="7" t="inlineStr">
+          <t>✅ ZI_Company_Name__c matches email domain, strengthening company identity.
+✅ ZI_Employees__c aligns with Enterprise segment, indicating a large company.
+⚠️ Website missing in ZoomInfo enrichment, reducing completeness.
+⚠️ LS_Company_Size_Range__c not provided, limiting validation of employee count.</t>
+        </is>
+      </c>
+      <c r="P28" s="10" t="inlineStr"/>
+      <c r="Q28" s="10" t="inlineStr"/>
+      <c r="R28" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1369,12 +1381,12 @@
     <row r="29" ht="25" customHeight="1">
       <c r="A29" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002Bmh1IUAR</t>
+          <t>00Q2H00002BmcWjUAJ</t>
         </is>
       </c>
       <c r="B29" s="7" t="inlineStr">
         <is>
-          <t>jshields@shieldslegal.com</t>
+          <t>ochoa_felipe_x@solarturbines.com</t>
         </is>
       </c>
       <c r="C29" s="7" t="inlineStr">
@@ -1387,29 +1399,33 @@
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="E29" s="7" t="n"/>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>1000+</t>
+        </is>
+      </c>
       <c r="F29" s="7" t="inlineStr">
         <is>
-          <t>shieldslegalgroup.com</t>
-        </is>
-      </c>
-      <c r="G29" s="7" t="n"/>
-      <c r="H29" s="7" t="inlineStr">
-        <is>
-          <t>Microsoft</t>
-        </is>
-      </c>
-      <c r="I29" s="7" t="n">
-        <v>210842</v>
-      </c>
-      <c r="J29" s="7" t="inlineStr">
-        <is>
-          <t>shieldslegal.com</t>
-        </is>
-      </c>
-      <c r="K29" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>www.caterpillar.com</t>
+        </is>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
+        <is>
+          <t>Caterpillar Inc.</t>
+        </is>
+      </c>
+      <c r="H29" s="7" t="n"/>
+      <c r="I29" s="7" t="inlineStr">
+        <is>
+          <t>Solar Turbines</t>
+        </is>
+      </c>
+      <c r="J29" s="7" t="n">
+        <v>8000</v>
+      </c>
+      <c r="K29" s="7" t="inlineStr">
+        <is>
+          <t>solarturbines.com</t>
         </is>
       </c>
       <c r="L29" s="8" t="inlineStr">
@@ -1417,31 +1433,24 @@
           <t>No</t>
         </is>
       </c>
-      <c r="M29" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="N29" s="10" t="inlineStr">
-        <is>
-          <t>❌ Company name 'Microsoft' conflicts with email domain 'shieldslegal.com'.
-⚠️ Employee count (210,842) significantly exceeds Enterprise segment size expectations.
-⚠️ Website inconsistency between lead-provided and enriched data.</t>
-        </is>
+      <c r="M29" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N29" s="9" t="n">
+        <v>60</v>
       </c>
       <c r="O29" s="10" t="inlineStr">
         <is>
-          <t>{
-  "ZI_Company_Name__c": "Shields Legal Group"
-}</t>
-        </is>
-      </c>
-      <c r="P29" s="10" t="inlineStr">
-        <is>
-          <t>{
-  "ZI_Employees__c": "100-250"
-}</t>
-        </is>
-      </c>
-      <c r="Q29" s="7" t="inlineStr">
+          <t>⚠️ ZI_Website__c and ZI_Company_Name__c do not match trusted data (Website, Company).
+✅ ZI_Employees__c (8000) aligns with LS_Company_Size_Range__c (1000+).
+⚠️ Large-company completeness check: ZI_Website__c missing despite high employee count.</t>
+        </is>
+      </c>
+      <c r="P29" s="10" t="inlineStr"/>
+      <c r="Q29" s="10" t="inlineStr"/>
+      <c r="R29" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1450,17 +1459,17 @@
     <row r="30" ht="25" customHeight="1">
       <c r="A30" s="7" t="inlineStr">
         <is>
-          <t>00Q2H00002BmhD6UAJ</t>
+          <t>00Q2H00002BmcxpUAB</t>
         </is>
       </c>
       <c r="B30" s="7" t="inlineStr">
         <is>
-          <t>skbennington@yahoo.com</t>
+          <t>rhoda.tamakloe@kaplanedfoundation.org</t>
         </is>
       </c>
       <c r="C30" s="7" t="inlineStr">
         <is>
-          <t>Affiliates</t>
+          <t>List Purchase</t>
         </is>
       </c>
       <c r="D30" s="7" t="inlineStr">
@@ -1470,46 +1479,63 @@
       </c>
       <c r="E30" s="7" t="inlineStr">
         <is>
-          <t>1000+</t>
-        </is>
-      </c>
-      <c r="F30" s="7" t="n"/>
-      <c r="G30" s="7" t="n"/>
-      <c r="H30" s="7" t="inlineStr">
-        <is>
-          <t>H&amp;R Block</t>
-        </is>
-      </c>
-      <c r="I30" s="7" t="n">
-        <v>46700</v>
-      </c>
-      <c r="J30" s="7" t="inlineStr">
-        <is>
-          <t>yahoo.com</t>
-        </is>
-      </c>
-      <c r="K30" s="8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L30" s="12" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="M30" s="11" t="n">
-        <v>50</v>
-      </c>
-      <c r="N30" s="10" t="inlineStr">
-        <is>
-          <t>❌ Large discrepancy in employee count (46700) and LS_Company_Size_Range__c (1000+).
-⚠️ Lead has a free email domain (yahoo.com) but enriched company is H&amp;R Block, raising authenticity concerns.</t>
-        </is>
-      </c>
-      <c r="O30" s="10" t="inlineStr"/>
+          <t>5000+</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>www.kaplan.com</t>
+        </is>
+      </c>
+      <c r="G30" s="7" t="inlineStr">
+        <is>
+          <t>Kaplan Educational Foundation</t>
+        </is>
+      </c>
+      <c r="H30" s="7" t="n"/>
+      <c r="I30" s="7" t="inlineStr">
+        <is>
+          <t>Kaplan</t>
+        </is>
+      </c>
+      <c r="J30" s="7" t="n">
+        <v>11900</v>
+      </c>
+      <c r="K30" s="7" t="inlineStr">
+        <is>
+          <t>kaplanedfoundation.org</t>
+        </is>
+      </c>
+      <c r="L30" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M30" s="8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N30" s="9" t="n">
+        <v>75</v>
+      </c>
+      <c r="O30" s="10" t="inlineStr">
+        <is>
+          <t>✅ ZI_Employees__c consistent with LS_Company_Size_Range__c and SegmentName.
+⚠️ ZI_Website__c and ZI_Company_Name__c are missing, impacting completeness.
+✅ Email domain matches Company and ZI_Company_Name__c, indicating consistency.
+⚠️ Website inferred from email domain; potential for accuracy issues.</t>
+        </is>
+      </c>
       <c r="P30" s="10" t="inlineStr"/>
-      <c r="Q30" s="7" t="inlineStr">
+      <c r="Q30" s="10" t="inlineStr">
+        <is>
+          <t>{
+  "ZI_Website__c": "kaplanedfoundation.org"
+}</t>
+        </is>
+      </c>
+      <c r="R30" s="7" t="inlineStr">
         <is>
           <t>success</t>
         </is>
@@ -1518,9 +1544,9 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A2:R2"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>